<commit_message>
Added functionality: Mark job as Faulted if the value for ShouldMarkJobAsFaulted is TRUE and an exception occurs in Initialization state (or Max consecutive system exceptions is reached and <> 0). Default value for ShouldMarkJobAsFaulted is FALSE.
</commit_message>
<xml_diff>
--- a/REFramework/VB/Data/Config.xlsx
+++ b/REFramework/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/UiPath/Reframework_update/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/StudioTemplates/REFramework/VB/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{13386E9B-2A6C-42D9-AD45-2092F6427BAE}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{860A6805-D6E9-485D-B8D3-B6A5A8C26AE0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10320" yWindow="17280" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
   </si>
   <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveRetryNumber is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
@@ -154,6 +151,15 @@
   </si>
   <si>
     <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
   </si>
 </sst>
 </file>
@@ -582,7 +588,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1614,7 +1620,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1670,15 +1676,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1751,55 +1757,65 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="28.8">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Aligning C# version with VB net version, adding consecutive SE counter in both versions and changing the condition for terminating the workflow for cases when an error happens before initializing the Config dictionary.
</commit_message>
<xml_diff>
--- a/REFramework/VB/Data/Config.xlsx
+++ b/REFramework/VB/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/StudioTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{860A6805-D6E9-485D-B8D3-B6A5A8C26AE0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10320" yWindow="17280" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was exceeded. </t>
-  </si>
-  <si>
     <t>ExceptionMessage_ConsecutiveErrors</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
 </sst>
 </file>
@@ -541,12 +541,12 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -588,13 +588,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1620,15 +1620,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1665,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1757,48 +1757,48 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2786,12 +2786,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated default Queue name in Config file from VB version to "ProcessABCQueue"
</commit_message>
<xml_diff>
--- a/REFramework/VB/Data/Config.xlsx
+++ b/REFramework/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\VB\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>ExceptionMessage_ConsecutiveErrors</t>
   </si>
   <si>
-    <t>TestFramework</t>
-  </si>
-  <si>
     <t>RetryNumberGetTransactionItem</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -537,16 +537,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -588,13 +588,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1619,16 +1619,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1665,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1760,45 +1760,45 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2786,12 +2786,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>